<commit_message>
add higher fO2 data to log(DU) vs log(fO2) plot
optional - uncomment lines in plot block
</commit_message>
<xml_diff>
--- a/Source_DvsfO2_Feb2025.xlsx
+++ b/Source_DvsfO2_Feb2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Documents/GitHub/DUDThZircon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6A1FDF-83EB-EE41-8064-8D981156DD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A9B2C4-7360-BE47-82CA-54F3D739962C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="23460" windowHeight="27000" xr2:uid="{3700DD82-4AF7-424A-B6E7-0BD72201019D}"/>
   </bookViews>
@@ -610,7 +610,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>